<commit_message>
add folder mobile test
</commit_message>
<xml_diff>
--- a/Excel/test-scenario.xlsx
+++ b/Excel/test-scenario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasmine/Katalon Studio/latihan-katalon/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C23FC9-11FE-804F-BD36-85AD11BEFCA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{378E99DA-05DA-484C-A059-88E85FC6D985}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="500" windowWidth="35840" windowHeight="20540" xr2:uid="{EDD54685-AAE0-0940-823F-BC0B0614D7F2}"/>
   </bookViews>
@@ -447,7 +447,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>